<commit_message>
docs(Hugo): add Hugo livequestion documentation
</commit_message>
<xml_diff>
--- a/hugo/dossier_fonctionnel/backlog.xlsx
+++ b/hugo/dossier_fonctionnel/backlog.xlsx
@@ -1,32 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iwn\private\portfolio\portfolio_v2\documentations\dossier_fonctionnel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\bts1\piscine3\documents\dossier_fonctionnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F22541-2E6F-4653-A0F4-0F75BA5F3BAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CA6738-22B8-453D-8383-BAF087E6D439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="750" windowWidth="18000" windowHeight="9360" xr2:uid="{939D4759-C654-4DEC-9B6D-EBCCDFC73002}"/>
+    <workbookView xWindow="2790" yWindow="750" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -35,88 +27,88 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
-    <t>Fonctionnalités</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Header Menu Animation</t>
-  </si>
-  <si>
-    <t>Scrollbar Progress</t>
-  </si>
-  <si>
-    <t>Darkmode Cookie</t>
-  </si>
-  <si>
-    <t>Project Diapositive</t>
-  </si>
-  <si>
-    <t>Formation Diapositive</t>
-  </si>
-  <si>
-    <t>Contact Form</t>
-  </si>
-  <si>
-    <t>Ajout Projet</t>
-  </si>
-  <si>
-    <t>Supprimer Projet</t>
-  </si>
-  <si>
-    <t>Modifier Projet</t>
-  </si>
-  <si>
-    <t>Consulter Message</t>
-  </si>
-  <si>
-    <t>Ajout Formation</t>
-  </si>
-  <si>
-    <t>Supprimer Formation</t>
-  </si>
-  <si>
-    <t>Modifier Formation</t>
-  </si>
-  <si>
-    <t>Mise en place d'un darkmode, enregistrer en cookie et prise en compte pref OS</t>
-  </si>
-  <si>
-    <t>Affichage de tout les projets stockés en base</t>
-  </si>
-  <si>
-    <t>Affichage de toutes les formations stockés en base</t>
-  </si>
-  <si>
-    <t>Formulaire de contact en bas de la page</t>
-  </si>
-  <si>
-    <t>Menu de navigation animer uniquement en css</t>
-  </si>
-  <si>
-    <t>Barre de progression remplaçant la scrollbar</t>
-  </si>
-  <si>
-    <t>Modification de projet depuis la page admin</t>
-  </si>
-  <si>
-    <t>Suppression de projet depuis la page admin</t>
-  </si>
-  <si>
-    <t>Suppression de formation depuis la page admin</t>
-  </si>
-  <si>
-    <t>Ajout de projet depuis la page admin</t>
-  </si>
-  <si>
-    <t>Ajout de formation depuis la page admin</t>
-  </si>
-  <si>
-    <t>Afficher les messages depuis l'espace admin</t>
-  </si>
-  <si>
-    <t>Modification de formation depuis la page admin</t>
+    <t>fonctionnalité</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>affiche l'ensemble des questions</t>
+  </si>
+  <si>
+    <t>ajouter question</t>
+  </si>
+  <si>
+    <t>ajouter une question en base de données</t>
+  </si>
+  <si>
+    <t>modification profil</t>
+  </si>
+  <si>
+    <t>inscription utilisateur</t>
+  </si>
+  <si>
+    <t>formulaire pour s'incrire</t>
+  </si>
+  <si>
+    <t>connexion utilisateur</t>
+  </si>
+  <si>
+    <t>formulaire pour se connecter</t>
+  </si>
+  <si>
+    <t>vue question</t>
+  </si>
+  <si>
+    <t>voir une question en fonction de son id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vue utilisateur </t>
+  </si>
+  <si>
+    <t>voir un utilisateur en fonction de son id</t>
+  </si>
+  <si>
+    <t>modifier ses données personnel</t>
+  </si>
+  <si>
+    <t>modification question</t>
+  </si>
+  <si>
+    <t>modifier une question</t>
+  </si>
+  <si>
+    <t>espace administrateur</t>
+  </si>
+  <si>
+    <t>back end pour gérer le site</t>
+  </si>
+  <si>
+    <t>question privé</t>
+  </si>
+  <si>
+    <t>question uniquement visible par ses amis</t>
+  </si>
+  <si>
+    <t>supprimer une question</t>
+  </si>
+  <si>
+    <t>permet de supprimer définitivement une question</t>
+  </si>
+  <si>
+    <t>supprimer utilisateur</t>
+  </si>
+  <si>
+    <t>permet de supprimer définitivement un utilisateur quand t-on est admin</t>
+  </si>
+  <si>
+    <t>supprimer son compte</t>
+  </si>
+  <si>
+    <t>permet de supprimer son compte</t>
+  </si>
+  <si>
+    <t>flux de questions</t>
   </si>
 </sst>
 </file>
@@ -172,7 +164,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -188,7 +180,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -200,7 +192,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -217,7 +209,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -247,29 +239,12 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -299,23 +274,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -467,17 +425,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{286A2AEE-3E66-4AA3-8869-775C5C791AA0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="71.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -488,13 +446,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -502,99 +459,98 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>